<commit_message>
Fix delete option for all facilities
</commit_message>
<xml_diff>
--- a/user_files/hilarytn/facility1/source2/line_8.xlsx
+++ b/user_files/hilarytn/facility1/source2/line_8.xlsx
@@ -58,13 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -510,7 +509,7 @@
           <t>9d072704-87a7-4a7a-9097-5cf366ad0b84</t>
         </is>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" t="n">
         <v>10</v>
       </c>
     </row>
@@ -544,7 +543,7 @@
           <t>9d072704-87a7-4a7a-9097-5cf366ad0b84</t>
         </is>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>